<commit_message>
[ENH] budget_plan invest construction now completed
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_plan_invest_construction_20180202.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_plan_invest_construction_20180202.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Construction Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t xml:space="preserve">Fiscal Year</t>
   </si>
@@ -105,13 +105,7 @@
     <t xml:space="preserve">Export Date</t>
   </si>
   <si>
-    <t xml:space="preserve">dd-mm-yyyy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Responsible by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Your name)</t>
   </si>
   <si>
     <t xml:space="preserve">Total Budget</t>
@@ -908,9 +902,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -925,8 +919,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -953,9 +947,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -970,8 +964,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,9 +992,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1015,8 +1009,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1043,9 +1037,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1060,8 +1054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1088,9 +1082,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1105,8 +1099,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,9 +1127,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1150,8 +1144,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1178,9 +1172,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1195,8 +1189,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1223,9 +1217,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1240,8 +1234,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1268,9 +1262,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -1285,8 +1279,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60120" y="64440"/>
-          <a:ext cx="7548120" cy="21260520"/>
+          <a:off x="60480" y="64800"/>
+          <a:ext cx="8333280" cy="21262680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1320,18 +1314,18 @@
   </sheetPr>
   <dimension ref="B1:AF30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="9" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="1" sqref="D5:F11 B10"/>
+      <selection pane="bottomRight" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.71"/>
@@ -1419,14 +1413,12 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1455,14 +1447,12 @@
       <c r="AD4" s="5"/>
       <c r="AE4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1493,7 +1483,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8" t="n">
@@ -1539,249 +1529,249 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="P7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="Q7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="R7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="S7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="T7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="U7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="10" t="s">
+      <c r="V7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="U7" s="10" t="s">
+      <c r="W7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="V7" s="10" t="s">
+      <c r="X7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="10" t="s">
+      <c r="Y7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="10" t="s">
+      <c r="Z7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Y7" s="10" t="s">
+      <c r="AA7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Z7" s="10" t="s">
+      <c r="AB7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AA7" s="10" t="s">
+      <c r="AC7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AB7" s="10" t="s">
+      <c r="AD7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AC7" s="10" t="s">
+      <c r="AF7" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="AD7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF7" s="12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="M8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="N8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="O8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="P8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="Q8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="14" t="s">
+      <c r="R8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="S8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="T8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="U8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="V8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="W8" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="X8" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="Y8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="X8" s="15" t="s">
+      <c r="Z8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Y8" s="15" t="s">
+      <c r="AA8" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="Z8" s="15" t="s">
+      <c r="AB8" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="AA8" s="15" t="s">
+      <c r="AC8" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="AB8" s="15" t="s">
+      <c r="AD8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AF8" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="AD8" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF8" s="16" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="G9" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="M9" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="N9" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="P9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="R9" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="P9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q9" s="14" t="s">
+      <c r="S9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="R9" s="14" t="s">
+      <c r="T9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="U9" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="T9" s="14" t="s">
+      <c r="V9" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="U9" s="14" t="s">
+      <c r="W9" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c r="X9" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="Y9" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="X9" s="15" t="s">
+      <c r="Z9" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="Y9" s="15" t="s">
+      <c r="AA9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="Z9" s="15" t="s">
+      <c r="AB9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="AA9" s="15" t="s">
+      <c r="AC9" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="AB9" s="15" t="s">
+      <c r="AD9" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="AC9" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD9" s="15" t="s">
-        <v>84</v>
-      </c>
       <c r="AF9" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="50.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1886,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="AD11" s="25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AE11" s="26"/>
       <c r="AF11" s="25" t="n">
@@ -3065,10 +3055,10 @@
   </sheetPr>
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B12" activeCellId="1" sqref="D5:F11 B12"/>
+      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3082,7 +3072,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="4.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3093,13 +3083,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="38" t="s">
         <v>37</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>